<commit_message>
Add voltage value to caps, update BOM, SCH, ASM
</commit_message>
<xml_diff>
--- a/work/HC-12 Work time.xlsx
+++ b/work/HC-12 Work time.xlsx
@@ -9,7 +9,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mhniuQajK+VVP+GfM99/kyH9oYLQQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mhZDiSQw4QYRMVf3MFuVh78jH7ymA=="/>
     </ext>
   </extLst>
 </workbook>
@@ -31,7 +31,7 @@
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="167" formatCode="d.m.yyyy"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -45,6 +45,11 @@
     <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -73,7 +78,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -106,6 +111,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="20" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="46" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
@@ -391,7 +402,7 @@
         <v>0.8597222222222223</v>
       </c>
       <c r="D6" s="3">
-        <f t="shared" ref="D6:D29" si="1">C6-B6</f>
+        <f t="shared" ref="D6:D30" si="1">C6-B6</f>
         <v>0.04722222222</v>
       </c>
     </row>
@@ -733,41 +744,54 @@
         <v>0.8402777777777778</v>
       </c>
       <c r="C29" s="11">
-        <v>0.8861111111111111</v>
+        <v>0.9076388888888889</v>
       </c>
       <c r="D29" s="3">
         <f t="shared" si="1"/>
-        <v>0.04583333333</v>
+        <v>0.06736111111</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="C30" s="6"/>
-      <c r="D30" s="12">
-        <f>SUM(D1:D29)</f>
-        <v>3.896527778</v>
+      <c r="A30" s="12">
+        <v>44839.0</v>
+      </c>
+      <c r="B30" s="13">
+        <v>0.8145833333333333</v>
+      </c>
+      <c r="C30" s="11">
+        <v>0.8930555555555556</v>
+      </c>
+      <c r="D30" s="3">
+        <f t="shared" si="1"/>
+        <v>0.07847222222</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="12">
+        <v>44840.0</v>
+      </c>
+      <c r="B31" s="13">
+        <v>0.84375</v>
+      </c>
       <c r="C31" s="6"/>
       <c r="D31" s="3"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="C32" s="6"/>
-      <c r="D32" s="3"/>
+      <c r="D32" s="14">
+        <f>SUM(D1:D30)</f>
+        <v>3.996527778</v>
+      </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="C33" s="6"/>
       <c r="D33" s="3"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
       <c r="C34" s="6"/>
       <c r="D34" s="3"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6"/>
       <c r="C35" s="6"/>
       <c r="D35" s="3"/>
     </row>
@@ -1941,8 +1965,18 @@
       <c r="C230" s="6"/>
       <c r="D230" s="3"/>
     </row>
-    <row r="231" ht="15.75" customHeight="1"/>
-    <row r="232" ht="15.75" customHeight="1"/>
+    <row r="231" ht="15.75" customHeight="1">
+      <c r="A231" s="6"/>
+      <c r="B231" s="6"/>
+      <c r="C231" s="6"/>
+      <c r="D231" s="3"/>
+    </row>
+    <row r="232" ht="15.75" customHeight="1">
+      <c r="A232" s="6"/>
+      <c r="B232" s="6"/>
+      <c r="C232" s="6"/>
+      <c r="D232" s="3"/>
+    </row>
     <row r="233" ht="15.75" customHeight="1"/>
     <row r="234" ht="15.75" customHeight="1"/>
     <row r="235" ht="15.75" customHeight="1"/>
@@ -2711,6 +2745,8 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
+    <row r="1002" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>